<commit_message>
Platform IO supporting files
</commit_message>
<xml_diff>
--- a/Arduino/Wireless buttons/Supporting Files/Box cover.xlsx
+++ b/Arduino/Wireless buttons/Supporting Files/Box cover.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\petla\source\repos\Scoreboard\Arduino\Wireless buttons\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\petla\source\repos\Scoreboard\Arduino\Wireless buttons\Supporting Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A6F251-8A71-42D4-823E-3DD47E72087A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92FD7B2C-C78C-47C0-ACA7-F9AC138D4BC4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{3A78579D-FDB4-4FDC-A9CA-2EA142ACB395}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$J$16</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$K$17</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -88,14 +88,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>40341</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:colOff>115042</xdr:colOff>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>266700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>72091</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:colOff>333556</xdr:colOff>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>196850</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -111,7 +111,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="40341" y="625288"/>
+          <a:off x="115042" y="625288"/>
           <a:ext cx="390338" cy="647327"/>
         </a:xfrm>
         <a:prstGeom prst="downArrow">
@@ -151,14 +151,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>40342</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:colOff>115043</xdr:colOff>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>72092</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:colOff>333557</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>349250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -174,7 +174,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="40342" y="1856441"/>
+          <a:off x="115043" y="1856441"/>
           <a:ext cx="390338" cy="644338"/>
         </a:xfrm>
         <a:prstGeom prst="downArrow">
@@ -213,15 +213,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>165100</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>266700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>196850</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>196850</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -276,15 +276,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>165100</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>196850</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>349250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -339,16 +339,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>279400</xdr:rowOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>354110</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>138210</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -363,8 +363,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1472453" y="637988"/>
-          <a:ext cx="383988" cy="501277"/>
+          <a:off x="1644276" y="809816"/>
+          <a:ext cx="383989" cy="501276"/>
           <a:chOff x="1600200" y="609600"/>
           <a:chExt cx="381000" cy="495300"/>
         </a:xfrm>
@@ -478,16 +478,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>176303</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>288731</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>271553</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:rowOff>295081</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -502,8 +502,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1295400" y="4324350"/>
-          <a:ext cx="806450" cy="361950"/>
+          <a:off x="1252068" y="4233202"/>
+          <a:ext cx="812426" cy="364938"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -546,15 +546,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>240924</xdr:colOff>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>279024</xdr:colOff>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -570,8 +570,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1352550" y="3670300"/>
-          <a:ext cx="749300" cy="304800"/>
+          <a:off x="1316689" y="3700182"/>
+          <a:ext cx="755276" cy="307789"/>
         </a:xfrm>
         <a:prstGeom prst="leftRightArrow">
           <a:avLst/>
@@ -607,15 +607,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>14943</xdr:colOff>
+      <xdr:colOff>59765</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>7473</xdr:rowOff>
+      <xdr:rowOff>29883</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>22413</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>104589</xdr:rowOff>
+      <xdr:colOff>328706</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>104590</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -630,8 +630,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14943" y="7473"/>
-          <a:ext cx="3593352" cy="5475940"/>
+          <a:off x="59765" y="29883"/>
+          <a:ext cx="3668059" cy="5550648"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -660,6 +660,140 @@
         <a:p>
           <a:pPr algn="l"/>
           <a:endParaRPr lang="cs-CZ" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>82173</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>67235</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>268941</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>82180</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="TextBox 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEEFB962-D803-4A59-8BFB-64DB42CECD1A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="440761" y="67235"/>
+          <a:ext cx="545356" cy="373533"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400" b="1"/>
+            <a:t>D</a:t>
+          </a:r>
+          <a:endParaRPr lang="cs-CZ" sz="2400" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>234568</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>62752</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>62747</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>77697</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="TextBox 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BB5107A-24B6-4BEB-86E1-B16591AD1535}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2386097" y="62752"/>
+          <a:ext cx="545356" cy="373533"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400" b="1"/>
+            <a:t>H</a:t>
+          </a:r>
+          <a:endParaRPr lang="cs-CZ" sz="2400" b="1"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -965,38 +1099,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12599052-A426-40A9-B22D-632165B79ED6}">
-  <dimension ref="A1:Q141"/>
+  <dimension ref="B1:R142"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="17" width="5" customWidth="1"/>
+    <col min="1" max="1" width="2.36328125" customWidth="1"/>
+    <col min="2" max="18" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-    </row>
-    <row r="2" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
+    <row r="1" spans="2:18" ht="7.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:18" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -1013,9 +1129,9 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
-    </row>
-    <row r="3" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1"/>
+      <c r="R2" s="1"/>
+    </row>
+    <row r="3" spans="2:18" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -1032,9 +1148,9 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
-    </row>
-    <row r="4" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1"/>
+      <c r="R3" s="1"/>
+    </row>
+    <row r="4" spans="2:18" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -1051,9 +1167,9 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
-    </row>
-    <row r="5" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
+      <c r="R4" s="1"/>
+    </row>
+    <row r="5" spans="2:18" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -1070,9 +1186,9 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
-    </row>
-    <row r="6" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
+      <c r="R5" s="1"/>
+    </row>
+    <row r="6" spans="2:18" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -1089,9 +1205,9 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-    </row>
-    <row r="7" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
+      <c r="R6" s="1"/>
+    </row>
+    <row r="7" spans="2:18" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -1108,9 +1224,9 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
-    </row>
-    <row r="8" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
+      <c r="R7" s="1"/>
+    </row>
+    <row r="8" spans="2:18" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -1127,9 +1243,9 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
-    </row>
-    <row r="9" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
+      <c r="R8" s="1"/>
+    </row>
+    <row r="9" spans="2:18" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1146,9 +1262,9 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
-    </row>
-    <row r="10" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="1"/>
+      <c r="R9" s="1"/>
+    </row>
+    <row r="10" spans="2:18" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1165,9 +1281,9 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
-    </row>
-    <row r="11" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="1"/>
+      <c r="R10" s="1"/>
+    </row>
+    <row r="11" spans="2:18" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -1184,9 +1300,9 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
-    </row>
-    <row r="12" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
+      <c r="R11" s="1"/>
+    </row>
+    <row r="12" spans="2:18" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -1203,9 +1319,9 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
-    </row>
-    <row r="13" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="1"/>
+      <c r="R12" s="1"/>
+    </row>
+    <row r="13" spans="2:18" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1222,9 +1338,9 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
-    </row>
-    <row r="14" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="1"/>
+      <c r="R13" s="1"/>
+    </row>
+    <row r="14" spans="2:18" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -1241,9 +1357,9 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
-    </row>
-    <row r="15" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="1"/>
+      <c r="R14" s="1"/>
+    </row>
+    <row r="15" spans="2:18" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -1260,9 +1376,9 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
-    </row>
-    <row r="16" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="1"/>
+      <c r="R15" s="1"/>
+    </row>
+    <row r="16" spans="2:18" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -1279,9 +1395,9 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
-    </row>
-    <row r="17" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="1"/>
+      <c r="R16" s="1"/>
+    </row>
+    <row r="17" spans="2:18" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -1298,9 +1414,9 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
-    </row>
-    <row r="18" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="1"/>
+      <c r="R17" s="1"/>
+    </row>
+    <row r="18" spans="2:18" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -1317,9 +1433,9 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
-    </row>
-    <row r="19" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="1"/>
+      <c r="R18" s="1"/>
+    </row>
+    <row r="19" spans="2:18" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1336,9 +1452,9 @@
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
-    </row>
-    <row r="20" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="1"/>
+      <c r="R19" s="1"/>
+    </row>
+    <row r="20" spans="2:18" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1355,9 +1471,9 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
-    </row>
-    <row r="21" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="1"/>
+      <c r="R20" s="1"/>
+    </row>
+    <row r="21" spans="2:18" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -1374,9 +1490,9 @@
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
-    </row>
-    <row r="22" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="1"/>
+      <c r="R21" s="1"/>
+    </row>
+    <row r="22" spans="2:18" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -1393,9 +1509,9 @@
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
-    </row>
-    <row r="23" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="1"/>
+      <c r="R22" s="1"/>
+    </row>
+    <row r="23" spans="2:18" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -1412,9 +1528,9 @@
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
-    </row>
-    <row r="24" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="1"/>
+      <c r="R23" s="1"/>
+    </row>
+    <row r="24" spans="2:18" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -1431,9 +1547,9 @@
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
-    </row>
-    <row r="25" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="1"/>
+      <c r="R24" s="1"/>
+    </row>
+    <row r="25" spans="2:18" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1450,9 +1566,9 @@
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
-    </row>
-    <row r="26" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="1"/>
+      <c r="R25" s="1"/>
+    </row>
+    <row r="26" spans="2:18" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -1469,13 +1585,32 @@
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
-    </row>
-    <row r="27" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="28" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="29" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="30" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="31" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="32" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+      <c r="R26" s="1"/>
+    </row>
+    <row r="27" spans="2:18" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+    </row>
+    <row r="28" spans="2:18" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="2:18" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="30" spans="2:18" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="31" spans="2:18" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="32" spans="2:18" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="33" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="34" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="35" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1585,6 +1720,7 @@
     <row r="139" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="140" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="141" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="142" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>